<commit_message>
Minor corrections made to the thesis.
</commit_message>
<xml_diff>
--- a/papers/ADFDPlus/ADFD+/ADFD+ vs Randoop.xlsx
+++ b/papers/ADFDPlus/ADFD+/ADFD+ vs Randoop.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22520" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="time1" sheetId="1" r:id="rId1"/>
     <sheet name="time" sheetId="2" r:id="rId2"/>
     <sheet name="no of tests" sheetId="3" r:id="rId3"/>
     <sheet name="Results" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="66">
   <si>
     <t>ADFD+</t>
   </si>
@@ -261,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +278,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -502,8 +509,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -520,8 +533,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -613,6 +630,9 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -704,6 +724,9 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -747,7 +770,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$41</c:f>
+              <c:f>time1!$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -766,7 +789,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$40:$E$40</c:f>
+              <c:f>time1!$D$40:$E$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -780,7 +803,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$41:$E$41</c:f>
+              <c:f>time1!$D$41:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -799,7 +822,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$42</c:f>
+              <c:f>time1!$C$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -824,7 +847,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$40:$E$40</c:f>
+              <c:f>time1!$D$40:$E$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -838,7 +861,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$42:$E$42</c:f>
+              <c:f>time1!$D$42:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -857,7 +880,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$43</c:f>
+              <c:f>time1!$C$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -869,7 +892,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$40:$E$40</c:f>
+              <c:f>time1!$D$40:$E$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -883,7 +906,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$43:$E$43</c:f>
+              <c:f>time1!$D$43:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -902,7 +925,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$44</c:f>
+              <c:f>time1!$C$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -918,7 +941,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$D$45:$E$45</c:f>
+                <c:f>time1!$D$45:$E$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -943,7 +966,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$40:$E$40</c:f>
+              <c:f>time1!$D$40:$E$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -957,7 +980,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$44:$E$44</c:f>
+              <c:f>time1!$D$44:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -981,11 +1004,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="618399864"/>
-        <c:axId val="618403064"/>
+        <c:axId val="2078776536"/>
+        <c:axId val="2133194952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="618399864"/>
+        <c:axId val="2078776536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +1017,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="618403064"/>
+        <c:crossAx val="2133194952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +1025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="618403064"/>
+        <c:axId val="2133194952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +1035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="618399864"/>
+        <c:crossAx val="2078776536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1207,11 +1230,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="614384888"/>
-        <c:axId val="614387864"/>
+        <c:axId val="2136592856"/>
+        <c:axId val="2136595832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614384888"/>
+        <c:axId val="2136592856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614387864"/>
+        <c:crossAx val="2136595832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1228,7 +1251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614387864"/>
+        <c:axId val="2136595832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1269,7 +1292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614384888"/>
+        <c:crossAx val="2136592856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,7 +1359,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$41</c:f>
+              <c:f>time1!$G$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1355,7 +1378,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$40:$I$40</c:f>
+              <c:f>time1!$H$40:$I$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1369,7 +1392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$41:$I$41</c:f>
+              <c:f>time1!$H$41:$I$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1388,7 +1411,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$42</c:f>
+              <c:f>time1!$G$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1413,7 +1436,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$40:$I$40</c:f>
+              <c:f>time1!$H$40:$I$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1427,7 +1450,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$42:$I$42</c:f>
+              <c:f>time1!$H$42:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1446,7 +1469,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$43</c:f>
+              <c:f>time1!$G$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1458,7 +1481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$40:$I$40</c:f>
+              <c:f>time1!$H$40:$I$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1472,7 +1495,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$43:$I$43</c:f>
+              <c:f>time1!$H$43:$I$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1491,7 +1514,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$44</c:f>
+              <c:f>time1!$G$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1507,7 +1530,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$H$45:$I$45</c:f>
+                <c:f>time1!$H$45:$I$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -1532,7 +1555,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$H$40:$I$40</c:f>
+              <c:f>time1!$H$40:$I$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1546,7 +1569,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$44:$I$44</c:f>
+              <c:f>time1!$H$44:$I$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1570,11 +1593,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614044728"/>
-        <c:axId val="614047928"/>
+        <c:axId val="2135183416"/>
+        <c:axId val="2135180200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614044728"/>
+        <c:axId val="2135183416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,7 +1606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614047928"/>
+        <c:crossAx val="2135180200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1591,7 +1614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614047928"/>
+        <c:axId val="2135180200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614044728"/>
+        <c:crossAx val="2135183416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1654,7 +1677,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$41</c:f>
+              <c:f>time1!$K$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1673,7 +1696,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$40:$M$40</c:f>
+              <c:f>time1!$L$40:$M$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1687,7 +1710,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$41:$M$41</c:f>
+              <c:f>time1!$L$41:$M$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1706,7 +1729,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$42</c:f>
+              <c:f>time1!$K$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1731,7 +1754,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$40:$M$40</c:f>
+              <c:f>time1!$L$40:$M$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1745,7 +1768,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$42:$M$42</c:f>
+              <c:f>time1!$L$42:$M$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1764,7 +1787,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$43</c:f>
+              <c:f>time1!$K$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1776,7 +1799,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$40:$M$40</c:f>
+              <c:f>time1!$L$40:$M$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1790,7 +1813,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$43:$M$43</c:f>
+              <c:f>time1!$L$43:$M$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1809,7 +1832,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$44</c:f>
+              <c:f>time1!$K$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1825,7 +1848,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$L$45:$M$45</c:f>
+                <c:f>time1!$L$45:$M$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -1850,7 +1873,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$40:$M$40</c:f>
+              <c:f>time1!$L$40:$M$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1864,7 +1887,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$44:$M$44</c:f>
+              <c:f>time1!$L$44:$M$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1888,11 +1911,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614084536"/>
-        <c:axId val="614087736"/>
+        <c:axId val="2135143544"/>
+        <c:axId val="2135140328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614084536"/>
+        <c:axId val="2135143544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614087736"/>
+        <c:crossAx val="2135140328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1909,7 +1932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614087736"/>
+        <c:axId val="2135140328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1919,7 +1942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614084536"/>
+        <c:crossAx val="2135143544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1962,7 +1985,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$41</c:f>
+              <c:f>time1!$O$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1981,7 +2004,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$40:$Q$40</c:f>
+              <c:f>time1!$P$40:$Q$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1995,7 +2018,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$41:$Q$41</c:f>
+              <c:f>time1!$P$41:$Q$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2014,7 +2037,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$42</c:f>
+              <c:f>time1!$O$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2039,7 +2062,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$40:$Q$40</c:f>
+              <c:f>time1!$P$40:$Q$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2053,7 +2076,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$42:$Q$42</c:f>
+              <c:f>time1!$P$42:$Q$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2072,7 +2095,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$43</c:f>
+              <c:f>time1!$O$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2084,7 +2107,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$40:$Q$40</c:f>
+              <c:f>time1!$P$40:$Q$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2098,7 +2121,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$43:$Q$43</c:f>
+              <c:f>time1!$P$43:$Q$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2117,7 +2140,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$44</c:f>
+              <c:f>time1!$O$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2133,7 +2156,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$P$45:$Q$45</c:f>
+                <c:f>time1!$P$45:$Q$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -2158,7 +2181,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$40:$Q$40</c:f>
+              <c:f>time1!$P$40:$Q$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2172,7 +2195,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$44:$Q$44</c:f>
+              <c:f>time1!$P$44:$Q$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2196,11 +2219,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614125128"/>
-        <c:axId val="614128328"/>
+        <c:axId val="2135103192"/>
+        <c:axId val="2135099976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614125128"/>
+        <c:axId val="2135103192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614128328"/>
+        <c:crossAx val="2135099976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2217,7 +2240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614128328"/>
+        <c:axId val="2135099976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,7 +2250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614125128"/>
+        <c:crossAx val="2135103192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2270,7 +2293,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$41</c:f>
+              <c:f>time1!$Y$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2289,7 +2312,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Z$40:$AA$40</c:f>
+              <c:f>time1!$Z$40:$AA$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2303,7 +2326,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$41:$AA$41</c:f>
+              <c:f>time1!$Z$41:$AA$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2322,7 +2345,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$42</c:f>
+              <c:f>time1!$Y$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2347,7 +2370,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Z$40:$AA$40</c:f>
+              <c:f>time1!$Z$40:$AA$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2361,7 +2384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$42:$AA$42</c:f>
+              <c:f>time1!$Z$42:$AA$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2380,7 +2403,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$43</c:f>
+              <c:f>time1!$Y$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2392,7 +2415,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Z$40:$AA$40</c:f>
+              <c:f>time1!$Z$40:$AA$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2406,7 +2429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$43:$AA$43</c:f>
+              <c:f>time1!$Z$43:$AA$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2425,7 +2448,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$44</c:f>
+              <c:f>time1!$Y$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2441,7 +2464,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$Z$44:$AA$44</c:f>
+                <c:f>time1!$Z$44:$AA$44</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -2466,7 +2489,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Z$40:$AA$40</c:f>
+              <c:f>time1!$Z$40:$AA$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2480,7 +2503,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$44:$AA$44</c:f>
+              <c:f>time1!$Z$44:$AA$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2504,11 +2527,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614166216"/>
-        <c:axId val="614169416"/>
+        <c:axId val="2135061848"/>
+        <c:axId val="2135058632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614166216"/>
+        <c:axId val="2135061848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2517,7 +2540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614169416"/>
+        <c:crossAx val="2135058632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2525,7 +2548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614169416"/>
+        <c:axId val="2135058632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2535,7 +2558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614166216"/>
+        <c:crossAx val="2135061848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2578,7 +2601,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$41</c:f>
+              <c:f>time1!$S$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2597,7 +2620,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$T$40:$U$40</c:f>
+              <c:f>time1!$T$40:$U$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2611,7 +2634,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$41:$U$41</c:f>
+              <c:f>time1!$T$41:$U$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2630,7 +2653,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$42</c:f>
+              <c:f>time1!$S$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2655,7 +2678,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$T$40:$U$40</c:f>
+              <c:f>time1!$T$40:$U$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2669,7 +2692,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$42:$U$42</c:f>
+              <c:f>time1!$T$42:$U$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2688,7 +2711,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$43</c:f>
+              <c:f>time1!$S$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2700,7 +2723,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$T$40:$U$40</c:f>
+              <c:f>time1!$T$40:$U$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2714,7 +2737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$43:$U$43</c:f>
+              <c:f>time1!$T$43:$U$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2733,7 +2756,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$44</c:f>
+              <c:f>time1!$S$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2749,7 +2772,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$T$45:$U$45</c:f>
+                <c:f>time1!$T$45:$U$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -2774,7 +2797,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$T$40:$U$40</c:f>
+              <c:f>time1!$T$40:$U$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -2788,7 +2811,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$44:$U$44</c:f>
+              <c:f>time1!$T$44:$U$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2812,11 +2835,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614207528"/>
-        <c:axId val="614210728"/>
+        <c:axId val="2135021144"/>
+        <c:axId val="2135017928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614207528"/>
+        <c:axId val="2135021144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2825,7 +2848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614210728"/>
+        <c:crossAx val="2135017928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2833,7 +2856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614210728"/>
+        <c:axId val="2135017928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2843,7 +2866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614207528"/>
+        <c:crossAx val="2135021144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3416,11 +3439,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614224888"/>
-        <c:axId val="614228120"/>
+        <c:axId val="2133142776"/>
+        <c:axId val="2133139528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614224888"/>
+        <c:axId val="2133142776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3439,7 +3462,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="614228120"/>
+        <c:crossAx val="2133139528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3447,7 +3470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614228120"/>
+        <c:axId val="2133139528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3469,13 +3492,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614224888"/>
+        <c:crossAx val="2133142776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4044,11 +4068,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="614311368"/>
-        <c:axId val="614314536"/>
+        <c:axId val="2134919400"/>
+        <c:axId val="2134916216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614311368"/>
+        <c:axId val="2134919400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4067,7 +4091,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="614314536"/>
+        <c:crossAx val="2134916216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4075,7 +4099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614314536"/>
+        <c:axId val="2134916216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4097,13 +4121,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614311368"/>
+        <c:crossAx val="2134919400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4298,11 +4323,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="614350520"/>
-        <c:axId val="614353496"/>
+        <c:axId val="2137482792"/>
+        <c:axId val="2137485768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614350520"/>
+        <c:axId val="2137482792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4311,7 +4336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614353496"/>
+        <c:crossAx val="2137485768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4319,7 +4344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614353496"/>
+        <c:axId val="2137485768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4360,7 +4385,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="614350520"/>
+        <c:crossAx val="2137482792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4586,8 +4611,8 @@
       <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1127760</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>690880</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>40640</xdr:rowOff>
     </xdr:to>
@@ -5035,8 +5060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:AJ72"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5045,36 +5070,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:27">
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="12"/>
       <c r="H1" s="10" t="s">
         <v>57</v>
       </c>
       <c r="I1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="10"/>
+      <c r="M1" s="12"/>
       <c r="P1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="Q1" s="10"/>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="10"/>
+      <c r="U1" s="12"/>
       <c r="Z1" s="10" t="s">
         <v>18</v>
       </c>
       <c r="AA1" s="10"/>
     </row>
     <row r="2" spans="4:27">
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -5083,10 +5108,10 @@
       <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="1" t="s">
@@ -5097,10 +5122,10 @@
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
@@ -6322,12 +6347,6 @@
       </c>
       <c r="I33" t="s">
         <v>1</v>
-      </c>
-      <c r="L33">
-        <v>3</v>
-      </c>
-      <c r="M33">
-        <v>84</v>
       </c>
       <c r="Z33" t="s">
         <v>0</v>
@@ -7251,7 +7270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="M35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="O46" activeCellId="5" sqref="E46 G46 I46 K46 M46 O46"/>
     </sheetView>
   </sheetViews>
@@ -9120,7 +9139,6 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -9134,8 +9152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="O48" activeCellId="5" sqref="E48 G48 I48 K48 M48 O48"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11001,7 +11019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I17:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
@@ -11189,7 +11207,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11197,4 +11214,533 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:O33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:15">
+      <c r="D1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="4:15">
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="4:15">
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>80</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="4:15">
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="4:15">
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>82</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>82</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15">
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>86</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15">
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>81</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="4:15">
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>77</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15">
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>92</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15">
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>87</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="4:15">
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>84</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="4:15">
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>79</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="4:15">
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>83</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="4:15">
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>81</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7">
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>82</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7">
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7">
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>78</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7">
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>93</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7">
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>86</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7">
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>85</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7">
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>82</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7">
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>74</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7">
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>81</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7">
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>83</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>84</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7">
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>85</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7">
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>86</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7">
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>89</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7">
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>81</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7">
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>